<commit_message>
changed photo edit logic
</commit_message>
<xml_diff>
--- a/Files/myContactSheet.xlsx
+++ b/Files/myContactSheet.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="118">
   <si>
     <t/>
   </si>
@@ -62,21 +62,54 @@
     <t>PHONENUMBER</t>
   </si>
   <si>
+    <t>78565371-E8C2-4C10-B4A4-0860073EE396</t>
+  </si>
+  <si>
+    <t>Mr</t>
+  </si>
+  <si>
+    <t>Ram</t>
+  </si>
+  <si>
+    <t>moorthy</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>2004-02-21</t>
+  </si>
+  <si>
+    <t>./Images/Uploads/men22.jpg</t>
+  </si>
+  <si>
+    <t>sda</t>
+  </si>
+  <si>
+    <t>sgdasgd</t>
+  </si>
+  <si>
+    <t>sgdsdga</t>
+  </si>
+  <si>
+    <t>sagag</t>
+  </si>
+  <si>
+    <t>sdgsa</t>
+  </si>
+  <si>
+    <t>ram123@gmail.com</t>
+  </si>
+  <si>
     <t>8C2D545C-6AA6-4AC9-889D-397EBD0609E6</t>
   </si>
   <si>
-    <t>Mr</t>
-  </si>
-  <si>
     <t>abhijith</t>
   </si>
   <si>
     <t>ff</t>
   </si>
   <si>
-    <t>male</t>
-  </si>
-  <si>
     <t>2005-12-05</t>
   </si>
   <si>
@@ -170,7 +203,7 @@
     <t>tech</t>
   </si>
   <si>
-    <t>1999-12-04</t>
+    <t>1999-12-09</t>
   </si>
   <si>
     <t>./Images/Uploads/men210.jpg</t>
@@ -278,46 +311,22 @@
     <t>tsvaishak@gmail.com</t>
   </si>
   <si>
-    <t>A21AC0C9-3EC6-4987-9F65-BA4C9DD731A4</t>
-  </si>
-  <si>
-    <t>Abhijith</t>
-  </si>
-  <si>
-    <t>techversant</t>
-  </si>
-  <si>
-    <t>2004-12-04</t>
-  </si>
-  <si>
-    <t>./Images/Uploads/men15.jpg</t>
-  </si>
-  <si>
-    <t>zx</t>
-  </si>
-  <si>
-    <t>gfsdasd</t>
+    <t>F0C33410-3CCB-43BF-82E2-E6C9DE4CF19D</t>
+  </si>
+  <si>
+    <t>jayasoorya</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>2001-12-04</t>
+  </si>
+  <si>
+    <t>./Images/Uploads/men415.jpg</t>
   </si>
   <si>
     <t>sdag</t>
-  </si>
-  <si>
-    <t>abhijithnaiju@techversantinfotech.com</t>
-  </si>
-  <si>
-    <t>F0C33410-3CCB-43BF-82E2-E6C9DE4CF19D</t>
-  </si>
-  <si>
-    <t>jayasoorya</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>2001-12-04</t>
-  </si>
-  <si>
-    <t>./Images/Uploads/men415.jpg</t>
   </si>
   <si>
     <t>sgda</t>
@@ -412,7 +421,7 @@
     <col min="14" max="14" width="37.30078125" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="5.734375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="11.52734375" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="11.6171875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="10.96484375" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="8.54296875" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="13.66796875" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="9.30859375" customWidth="true" bestFit="true"/>
@@ -509,13 +518,13 @@
         <v>27</v>
       </c>
       <c r="M2" t="n">
-        <v>65754.0</v>
+        <v>64456.0</v>
       </c>
       <c r="N2" t="s">
         <v>28</v>
       </c>
       <c r="O2" t="n">
-        <v>6.5467666E7</v>
+        <v>9.746829901E9</v>
       </c>
     </row>
     <row r="3">
@@ -523,46 +532,46 @@
         <v>29</v>
       </c>
       <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
         <v>30</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>31</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" t="s">
         <v>32</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>33</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>34</v>
       </c>
-      <c r="G3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>35</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>36</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>37</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>38</v>
       </c>
-      <c r="L3" t="s">
-        <v>27</v>
-      </c>
       <c r="M3" t="n">
-        <v>4334.0</v>
+        <v>65754.0</v>
       </c>
       <c r="N3" t="s">
         <v>39</v>
       </c>
       <c r="O3" t="n">
-        <v>6.85578123E8</v>
+        <v>6.5467666E7</v>
       </c>
     </row>
     <row r="4">
@@ -570,93 +579,93 @@
         <v>40</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="F4" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="G4" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="H4" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="I4" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="J4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="K4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="L4" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="M4" t="n">
-        <v>4366.0</v>
+        <v>4334.0</v>
       </c>
       <c r="N4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="O4" t="n">
-        <v>3.64747737E8</v>
+        <v>6.85578123E8</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
         <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E5" t="s">
         <v>20</v>
       </c>
       <c r="F5" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="G5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="K5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="L5" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="M5" t="n">
-        <v>695505.0</v>
+        <v>4366.0</v>
       </c>
       <c r="N5" t="s">
         <v>59</v>
       </c>
       <c r="O5" t="n">
-        <v>9.746829901E9</v>
+        <v>3.64747737E8</v>
       </c>
     </row>
     <row r="6">
@@ -703,7 +712,7 @@
         <v>70</v>
       </c>
       <c r="O6" t="n">
-        <v>7.87999777E8</v>
+        <v>9.746829901E9</v>
       </c>
     </row>
     <row r="7">
@@ -738,157 +747,157 @@
         <v>78</v>
       </c>
       <c r="K7" t="s">
-        <v>38</v>
+        <v>79</v>
       </c>
       <c r="L7" t="s">
-        <v>27</v>
+        <v>80</v>
       </c>
       <c r="M7" t="n">
         <v>695505.0</v>
       </c>
       <c r="N7" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="O7" t="n">
-        <v>9.746829901E9</v>
+        <v>7.87999777E8</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B8" t="s">
         <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>84</v>
       </c>
       <c r="E8" t="s">
         <v>20</v>
       </c>
       <c r="F8" t="s">
-        <v>34</v>
+        <v>85</v>
       </c>
       <c r="G8" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="H8" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="I8" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="J8" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="K8" t="s">
-        <v>86</v>
+        <v>49</v>
       </c>
       <c r="L8" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="M8" t="n">
-        <v>65754.0</v>
+        <v>695505.0</v>
       </c>
       <c r="N8" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="O8" t="n">
-        <v>5457457.0</v>
+        <v>9.746829901E9</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B9" t="s">
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D9" t="s">
-        <v>90</v>
+        <v>53</v>
       </c>
       <c r="E9" t="s">
         <v>20</v>
       </c>
       <c r="F9" t="s">
-        <v>91</v>
+        <v>45</v>
       </c>
       <c r="G9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I9" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="J9" t="s">
-        <v>35</v>
+        <v>96</v>
       </c>
       <c r="K9" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="L9" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="M9" t="n">
-        <v>4533.0</v>
+        <v>65754.0</v>
       </c>
       <c r="N9" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="O9" t="n">
-        <v>1.112222333E9</v>
+        <v>5457457.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B10" t="s">
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D10" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E10" t="s">
         <v>20</v>
       </c>
       <c r="F10" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="G10" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="H10" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="I10" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="J10" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="K10" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="L10" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="M10" t="n">
         <v>45757.0</v>
       </c>
       <c r="N10" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="O10" t="n">
         <v>1122233.0</v>
@@ -896,46 +905,46 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B11" t="s">
         <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D11" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="E11" t="s">
         <v>20</v>
       </c>
       <c r="F11" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="G11" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="H11" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="I11" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="J11" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="K11" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="L11" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="M11" t="n">
         <v>695505.0</v>
       </c>
       <c r="N11" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="O11" t="n">
         <v>6.3463646E7</v>

</xml_diff>

<commit_message>
latest review changes 12/12
</commit_message>
<xml_diff>
--- a/Files/myContactSheet.xlsx
+++ b/Files/myContactSheet.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="43">
   <si>
     <t/>
   </si>
@@ -65,40 +65,82 @@
     <t>ROLES</t>
   </si>
   <si>
+    <t>Miss</t>
+  </si>
+  <si>
+    <t>gopika</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>2000-04-28</t>
+  </si>
+  <si>
+    <t>./Images/Uploads/girl112.jpg</t>
+  </si>
+  <si>
+    <t>rtys</t>
+  </si>
+  <si>
+    <t>jgjf</t>
+  </si>
+  <si>
+    <t>Thiruvananthapuram</t>
+  </si>
+  <si>
+    <t>Kerala</t>
+  </si>
+  <si>
+    <t>Indian</t>
+  </si>
+  <si>
+    <t>gopika123@gmail.com</t>
+  </si>
+  <si>
+    <t>Student, Relative</t>
+  </si>
+  <si>
     <t>Mr</t>
   </si>
   <si>
-    <t>Ram</t>
-  </si>
-  <si>
-    <t>raj</t>
+    <t>abhijith</t>
+  </si>
+  <si>
+    <t>ff</t>
   </si>
   <si>
     <t>male</t>
   </si>
   <si>
-    <t>2009-05-05</t>
-  </si>
-  <si>
-    <t>./Images/Uploads/men345.jpg</t>
-  </si>
-  <si>
-    <t>ghjg</t>
-  </si>
-  <si>
-    <t>ghjhf</t>
-  </si>
-  <si>
-    <t>Kerala</t>
-  </si>
-  <si>
-    <t>Indian</t>
-  </si>
-  <si>
-    <t>ram123@gmail.com</t>
-  </si>
-  <si>
-    <t>Admin, Student</t>
+    <t>2006-02-05</t>
+  </si>
+  <si>
+    <t>./Images/Uploads/men219.jpg</t>
+  </si>
+  <si>
+    <t>fghfgh</t>
+  </si>
+  <si>
+    <t>gffgh</t>
+  </si>
+  <si>
+    <t>fgh</t>
+  </si>
+  <si>
+    <t>fghsjf</t>
+  </si>
+  <si>
+    <t>jfgj</t>
+  </si>
+  <si>
+    <t>abhijithff59@gmail.com</t>
+  </si>
+  <si>
+    <t>Admin, Guest</t>
   </si>
 </sst>
 </file>
@@ -143,15 +185,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="7" max="7" width="28.42578125" customWidth="true" bestFit="true"/>
-    <col min="14" max="14" width="19.1875" customWidth="true" bestFit="true"/>
-    <col min="16" max="16" width="14.9765625" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="19.94140625" customWidth="true" bestFit="true"/>
+    <col min="14" max="14" width="22.6328125" customWidth="true" bestFit="true"/>
+    <col min="16" max="16" width="16.30859375" customWidth="true" bestFit="true"/>
     <col min="1" max="1" width="11.5859375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="5.734375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="11.52734375" customWidth="true" bestFit="true"/>
@@ -160,7 +203,6 @@
     <col min="6" max="6" width="13.66796875" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="9.30859375" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="7.53515625" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="9.0234375" customWidth="true" bestFit="true"/>
     <col min="11" max="11" width="6.65625" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="13.12890625" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="9.20703125" customWidth="true" bestFit="true"/>
@@ -219,7 +261,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>13.0</v>
+        <v>16.0</v>
       </c>
       <c r="B2" t="s">
         <v>17</v>
@@ -246,25 +288,75 @@
         <v>24</v>
       </c>
       <c r="J2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M2" t="n">
+        <v>75547.0</v>
+      </c>
+      <c r="N2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" t="n">
+        <v>6.546766666E9</v>
+      </c>
+      <c r="P2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3" t="s">
+        <v>39</v>
+      </c>
+      <c r="L3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M3" t="n">
         <v>695505.0</v>
       </c>
-      <c r="N2" t="s">
-        <v>27</v>
-      </c>
-      <c r="O2" t="n">
+      <c r="N3" t="s">
+        <v>41</v>
+      </c>
+      <c r="O3" t="n">
         <v>9.746829901E9</v>
       </c>
-      <c r="P2" t="s">
-        <v>28</v>
+      <c r="P3" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
latest review changes 13/12
</commit_message>
<xml_diff>
--- a/Files/myContactSheet.xlsx
+++ b/Files/myContactSheet.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="53">
   <si>
     <t/>
   </si>
@@ -65,82 +65,112 @@
     <t>ROLES</t>
   </si>
   <si>
+    <t>Mr</t>
+  </si>
+  <si>
+    <t>abhijith</t>
+  </si>
+  <si>
+    <t>ff</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>2000-12-13</t>
+  </si>
+  <si>
+    <t>./Images/Uploads/men45.jpg</t>
+  </si>
+  <si>
+    <t>fdzsfj</t>
+  </si>
+  <si>
+    <t>jszdfijsd</t>
+  </si>
+  <si>
+    <t>Sujfds</t>
+  </si>
+  <si>
+    <t>jsfdyxh</t>
+  </si>
+  <si>
+    <t>dfhsayd</t>
+  </si>
+  <si>
+    <t>abhijithff59@gmail.com</t>
+  </si>
+  <si>
+    <t>Guest</t>
+  </si>
+  <si>
+    <t>Dinil</t>
+  </si>
+  <si>
+    <t>thomas</t>
+  </si>
+  <si>
+    <t>2002-05-16</t>
+  </si>
+  <si>
+    <t>./Images/Uploads/men2.jpg</t>
+  </si>
+  <si>
+    <t>dfajfgkj</t>
+  </si>
+  <si>
+    <t>adfjfgjk</t>
+  </si>
+  <si>
+    <t>vhxcz</t>
+  </si>
+  <si>
+    <t>fxgjhdz</t>
+  </si>
+  <si>
+    <t>xzm</t>
+  </si>
+  <si>
+    <t>dinilthomas@techversantinfotech.com</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
     <t>Miss</t>
   </si>
   <si>
-    <t>gopika</t>
-  </si>
-  <si>
-    <t>s</t>
+    <t>Malavika</t>
   </si>
   <si>
     <t>female</t>
   </si>
   <si>
-    <t>2000-04-28</t>
-  </si>
-  <si>
-    <t>./Images/Uploads/girl112.jpg</t>
-  </si>
-  <si>
-    <t>rtys</t>
-  </si>
-  <si>
-    <t>jgjf</t>
-  </si>
-  <si>
-    <t>Thiruvananthapuram</t>
-  </si>
-  <si>
-    <t>Kerala</t>
-  </si>
-  <si>
-    <t>Indian</t>
-  </si>
-  <si>
-    <t>gopika123@gmail.com</t>
-  </si>
-  <si>
-    <t>Student, Relative</t>
-  </si>
-  <si>
-    <t>Mr</t>
-  </si>
-  <si>
-    <t>abhijith</t>
-  </si>
-  <si>
-    <t>ff</t>
-  </si>
-  <si>
-    <t>male</t>
-  </si>
-  <si>
-    <t>2006-02-05</t>
-  </si>
-  <si>
-    <t>./Images/Uploads/men219.jpg</t>
-  </si>
-  <si>
-    <t>fghfgh</t>
-  </si>
-  <si>
-    <t>gffgh</t>
-  </si>
-  <si>
-    <t>fgh</t>
-  </si>
-  <si>
-    <t>fghsjf</t>
-  </si>
-  <si>
-    <t>jfgj</t>
-  </si>
-  <si>
-    <t>abhijithff59@gmail.com</t>
-  </si>
-  <si>
-    <t>Admin, Guest</t>
+    <t>2000-09-05</t>
+  </si>
+  <si>
+    <t>./Images/Uploads/girl1.jpg</t>
+  </si>
+  <si>
+    <t>sdhdfaj</t>
+  </si>
+  <si>
+    <t>sdsAhy</t>
+  </si>
+  <si>
+    <t>sDJgcfxdc</t>
+  </si>
+  <si>
+    <t>fxdzh</t>
+  </si>
+  <si>
+    <t>SDhjxghcfdz</t>
+  </si>
+  <si>
+    <t>malu123@gmail.com</t>
+  </si>
+  <si>
+    <t>Admin, Student</t>
   </si>
 </sst>
 </file>
@@ -185,16 +215,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="7" max="7" width="28.42578125" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="19.94140625" customWidth="true" bestFit="true"/>
-    <col min="14" max="14" width="22.6328125" customWidth="true" bestFit="true"/>
-    <col min="16" max="16" width="16.30859375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="27.3125" customWidth="true" bestFit="true"/>
+    <col min="14" max="14" width="35.94921875" customWidth="true" bestFit="true"/>
+    <col min="16" max="16" width="14.9765625" customWidth="true" bestFit="true"/>
     <col min="1" max="1" width="11.5859375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="5.734375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="11.52734375" customWidth="true" bestFit="true"/>
@@ -202,8 +231,9 @@
     <col min="5" max="5" width="8.54296875" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="13.66796875" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="9.30859375" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="7.53515625" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="6.65625" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="8.16796875" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="9.62890625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="7.40625" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="13.12890625" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="9.20703125" customWidth="true" bestFit="true"/>
     <col min="15" max="15" width="15.671875" customWidth="true" bestFit="true"/>
@@ -261,7 +291,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>16.0</v>
+        <v>25.0</v>
       </c>
       <c r="B2" t="s">
         <v>17</v>
@@ -297,13 +327,13 @@
         <v>27</v>
       </c>
       <c r="M2" t="n">
-        <v>75547.0</v>
+        <v>755476.0</v>
       </c>
       <c r="N2" t="s">
         <v>28</v>
       </c>
       <c r="O2" t="n">
-        <v>6.546766666E9</v>
+        <v>9.746829901E9</v>
       </c>
       <c r="P2" t="s">
         <v>29</v>
@@ -311,52 +341,102 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>17.0</v>
+        <v>26.0</v>
       </c>
       <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
         <v>30</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>31</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" t="s">
         <v>32</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>33</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>34</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>35</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
         <v>36</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>37</v>
       </c>
-      <c r="J3" t="s">
+      <c r="L3" t="s">
         <v>38</v>
       </c>
-      <c r="K3" t="s">
+      <c r="M3" t="n">
+        <v>433465.0</v>
+      </c>
+      <c r="N3" t="s">
         <v>39</v>
       </c>
-      <c r="L3" t="s">
+      <c r="O3" t="n">
+        <v>7.854874571E9</v>
+      </c>
+      <c r="P3" t="s">
         <v>40</v>
       </c>
-      <c r="M3" t="n">
-        <v>695505.0</v>
-      </c>
-      <c r="N3" t="s">
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="B4" t="s">
         <v>41</v>
       </c>
-      <c r="O3" t="n">
-        <v>9.746829901E9</v>
-      </c>
-      <c r="P3" t="s">
+      <c r="C4" t="s">
         <v>42</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J4" t="s">
+        <v>48</v>
+      </c>
+      <c r="K4" t="s">
+        <v>49</v>
+      </c>
+      <c r="L4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M4" t="n">
+        <v>5436765.0</v>
+      </c>
+      <c r="N4" t="s">
+        <v>51</v>
+      </c>
+      <c r="O4" t="n">
+        <v>3.567878545E9</v>
+      </c>
+      <c r="P4" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>